<commit_message>
update `caravel-dev-v5-M.2` BOM with M.2 connector
</commit_message>
<xml_diff>
--- a/hardware/caravel-dev-v5-M.2/caravel-dev-v5-M.2.xlsx
+++ b/hardware/caravel-dev-v5-M.2/caravel-dev-v5-M.2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Efabless\caravel_board\hardware\caravel_pcb_v4_FTDI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Efabless\caravel_board\hardware\caravel-dev-v5-M.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41750F50-E64B-42E4-AE33-63720122C312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A45909-5D17-42DA-9725-BFFF586065C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2960" yWindow="2960" windowWidth="19200" windowHeight="11170" xr2:uid="{DBB590BE-7B6D-5543-BF5E-2321E179B520}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{DBB590BE-7B6D-5543-BF5E-2321E179B520}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="3" r:id="rId1"/>
@@ -36,9 +36,6 @@
     <t>U6</t>
   </si>
   <si>
-    <t>Caravel</t>
-  </si>
-  <si>
     <t>U1</t>
   </si>
   <si>
@@ -75,9 +72,6 @@
     <t>Designators</t>
   </si>
   <si>
-    <t>EF</t>
-  </si>
-  <si>
     <t>DK</t>
   </si>
   <si>
@@ -205,6 +199,12 @@
   </si>
   <si>
     <t>TAR5S16UTE85LF</t>
+  </si>
+  <si>
+    <t>M.2 E connector</t>
+  </si>
+  <si>
+    <t>SparkFun</t>
   </si>
 </sst>
 </file>
@@ -291,10 +291,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -302,9 +301,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -315,7 +311,6 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -635,355 +630,346 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="27.33203125" customWidth="1"/>
-    <col min="2" max="2" width="6.33203125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" style="5" customWidth="1"/>
     <col min="4" max="4" width="33" customWidth="1"/>
     <col min="6" max="6" width="13.58203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="5" t="s">
         <v>12</v>
       </c>
+      <c r="B1" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="5">
+        <v>2</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="6">
+      <c r="F3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="5">
         <v>1</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="3" t="s">
+      <c r="D4" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="5">
+        <v>1</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="6"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="6">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="6">
+      <c r="B7" s="5">
         <v>1</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="2" t="s">
+      <c r="D7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B8" s="5">
         <v>1</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="7">
-        <v>1</v>
-      </c>
-      <c r="D6" s="8" t="s">
+      <c r="D8" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" t="s">
         <v>57</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="8"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="6">
-        <v>1</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8" s="6">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" s="7">
+        <v>40</v>
+      </c>
+      <c r="B9" s="5">
         <v>4</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>36</v>
+      <c r="D9" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="E9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>53</v>
-      </c>
-      <c r="B10" s="7">
+        <v>51</v>
+      </c>
+      <c r="B10" s="5">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>17</v>
+        <v>14</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="5">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="7">
-        <v>2</v>
-      </c>
-      <c r="C11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>56</v>
-      </c>
       <c r="E11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>55</v>
-      </c>
-      <c r="B12" s="7">
+        <v>53</v>
+      </c>
+      <c r="B12" s="5">
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="E12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>52</v>
-      </c>
-      <c r="B13" s="7">
+        <v>50</v>
+      </c>
+      <c r="B13" s="5">
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>21</v>
+        <v>18</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="E13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14" s="7">
+        <v>45</v>
+      </c>
+      <c r="B14" s="5">
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="E14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" s="7">
+        <v>38</v>
+      </c>
+      <c r="B15" s="5">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>35</v>
+        <v>22</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="E15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="7">
+        <v>39</v>
+      </c>
+      <c r="B16" s="5">
         <v>2</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="3">
         <v>150</v>
       </c>
-      <c r="D16" s="8" t="s">
-        <v>25</v>
+      <c r="D16" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="E16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="7">
+        <v>41</v>
+      </c>
+      <c r="B17" s="5">
         <v>2</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="3">
         <v>82</v>
       </c>
-      <c r="D17" s="9" t="s">
-        <v>26</v>
+      <c r="D17" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="E17" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="7">
+        <v>5</v>
+      </c>
+      <c r="B18" s="5">
         <v>1</v>
       </c>
-      <c r="D18" s="8" t="s">
-        <v>31</v>
+      <c r="D18" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="E18" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B19" s="7">
+        <v>2</v>
+      </c>
+      <c r="B19" s="5">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="10" t="s">
         <v>32</v>
       </c>
+      <c r="D19" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="E19" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="5">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="7">
-        <v>1</v>
-      </c>
-      <c r="C20" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>5</v>
-      </c>
       <c r="E20" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" s="7">
+        <v>42</v>
+      </c>
+      <c r="B21" s="5">
         <v>2</v>
       </c>
-      <c r="D21" s="10" t="s">
-        <v>45</v>
+      <c r="D21" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="E21" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1006,8 +992,9 @@
     <hyperlink ref="D5" r:id="rId16" xr:uid="{4A73DBD0-B5FB-4EA1-A7E5-13DF03ABC85B}"/>
     <hyperlink ref="D10" r:id="rId17" xr:uid="{E464CA61-42F7-44EB-BF01-8B800CA45EF3}"/>
     <hyperlink ref="D11" r:id="rId18" xr:uid="{BD6CFC13-E75A-43AB-8083-A44296ED7D4B}"/>
+    <hyperlink ref="D8" r:id="rId19" xr:uid="{56DDA58F-65D3-4331-9638-21803D3C06A9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId19"/>
+  <pageSetup orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>